<commit_message>
i have done automation scripts on functional scenarios of shop page
</commit_message>
<xml_diff>
--- a/ecommerse_automation_gurupreeth/project_documents_ANUSHA_shopPage.xlsx
+++ b/ecommerse_automation_gurupreeth/project_documents_ANUSHA_shopPage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\ECODERS_TESTING_FOLDER\project_management_tool_jira\ecommerse_automation_gurupreeth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9488DBD4-BAFA-4A0A-926D-881EF5BD2848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA44153E-6784-4442-985A-C721E547B15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="300" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="550">
   <si>
     <t>header elements</t>
   </si>
@@ -938,12 +938,6 @@
   </si>
   <si>
     <t>Shop | ECODERS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title </t>
-  </si>
-  <si>
-    <t>url</t>
   </si>
   <si>
     <t>localhost:5173/shop</t>
@@ -1699,6 +1693,15 @@
   </si>
   <si>
     <t>Search-Products | ECODERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home | ECODERS </t>
+  </si>
+  <si>
+    <t>Wishlist | ECODERS</t>
+  </si>
+  <si>
+    <t>Login | ECODERS</t>
   </si>
 </sst>
 </file>
@@ -3032,10 +3035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3047,1044 +3050,1051 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>304</v>
+        <v>547</v>
       </c>
       <c r="B2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D14" t="s">
         <v>308</v>
-      </c>
-      <c r="B4" t="s">
-        <v>309</v>
-      </c>
-      <c r="D4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>311</v>
-      </c>
-      <c r="D5" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>313</v>
-      </c>
-      <c r="D6" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>315</v>
-      </c>
-      <c r="D7" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>317</v>
-      </c>
-      <c r="D8" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>319</v>
-      </c>
-      <c r="D9" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>321</v>
-      </c>
-      <c r="D11" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>323</v>
-      </c>
-      <c r="D12" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>325</v>
-      </c>
-      <c r="D13" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>327</v>
-      </c>
-      <c r="D14" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="D15" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="D16" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="D17" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="D18" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="D19" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>339</v>
-      </c>
-      <c r="D20" t="s">
-        <v>340</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
       <c r="D21" t="s">
-        <v>342</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>321</v>
+      </c>
+      <c r="D22" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>323</v>
+      </c>
+      <c r="D23" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>325</v>
+      </c>
+      <c r="D24" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>327</v>
+      </c>
+      <c r="D25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>329</v>
+      </c>
+      <c r="D26" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>331</v>
+      </c>
+      <c r="D27" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>333</v>
+      </c>
+      <c r="D28" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>335</v>
+      </c>
+      <c r="D29" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>337</v>
+      </c>
+      <c r="D30" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>339</v>
+      </c>
+      <c r="D31" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
-        <v>343</v>
-      </c>
-      <c r="D22" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>345</v>
-      </c>
-      <c r="D23" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>347</v>
-      </c>
-      <c r="D24" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>349</v>
-      </c>
-      <c r="D25" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>351</v>
-      </c>
-      <c r="D26" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>353</v>
-      </c>
-      <c r="D27" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>355</v>
-      </c>
-      <c r="D28" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>357</v>
-      </c>
-      <c r="D29" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>359</v>
-      </c>
-      <c r="D30" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>361</v>
-      </c>
-      <c r="D31" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="D32" t="s">
-        <v>364</v>
+        <v>342</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="D33" t="s">
-        <v>366</v>
+        <v>344</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>367</v>
+        <v>345</v>
       </c>
       <c r="D34" t="s">
-        <v>368</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="D35" t="s">
-        <v>370</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>371</v>
+        <v>349</v>
       </c>
       <c r="D36" t="s">
-        <v>372</v>
+        <v>350</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>373</v>
+        <v>351</v>
       </c>
       <c r="D37" t="s">
-        <v>374</v>
+        <v>352</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>375</v>
+        <v>353</v>
       </c>
       <c r="D38" t="s">
-        <v>376</v>
+        <v>354</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>377</v>
+        <v>355</v>
       </c>
       <c r="D39" t="s">
-        <v>378</v>
+        <v>356</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>379</v>
+        <v>357</v>
       </c>
       <c r="D40" t="s">
-        <v>380</v>
+        <v>358</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>381</v>
+        <v>359</v>
       </c>
       <c r="D41" t="s">
-        <v>382</v>
+        <v>360</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="D42" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="D43" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>387</v>
+        <v>365</v>
       </c>
       <c r="D44" t="s">
-        <v>388</v>
+        <v>366</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>389</v>
+        <v>367</v>
       </c>
       <c r="D45" t="s">
-        <v>390</v>
+        <v>368</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>391</v>
+        <v>369</v>
       </c>
       <c r="D46" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>393</v>
+        <v>371</v>
       </c>
       <c r="D47" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>395</v>
+        <v>373</v>
       </c>
       <c r="D48" t="s">
-        <v>396</v>
+        <v>374</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>397</v>
+        <v>375</v>
       </c>
       <c r="D49" t="s">
-        <v>398</v>
+        <v>376</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>399</v>
+        <v>377</v>
       </c>
       <c r="D50" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>401</v>
+        <v>379</v>
       </c>
       <c r="D51" t="s">
-        <v>402</v>
+        <v>380</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
       <c r="D52" t="s">
-        <v>404</v>
+        <v>382</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>405</v>
+        <v>383</v>
       </c>
       <c r="D53" t="s">
-        <v>406</v>
+        <v>384</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
       <c r="D54" t="s">
-        <v>408</v>
+        <v>386</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>409</v>
+        <v>387</v>
       </c>
       <c r="D55" t="s">
-        <v>410</v>
+        <v>388</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D56" t="s">
-        <v>412</v>
+        <v>390</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>413</v>
+        <v>391</v>
       </c>
       <c r="D57" t="s">
-        <v>414</v>
+        <v>392</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>415</v>
+        <v>393</v>
       </c>
       <c r="D58" t="s">
-        <v>416</v>
+        <v>394</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>417</v>
+        <v>395</v>
       </c>
       <c r="D59" t="s">
-        <v>418</v>
+        <v>396</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>419</v>
+        <v>397</v>
       </c>
       <c r="D60" t="s">
-        <v>420</v>
+        <v>398</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="D61" t="s">
-        <v>422</v>
+        <v>400</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>423</v>
+        <v>401</v>
       </c>
       <c r="D62" t="s">
-        <v>424</v>
+        <v>402</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>425</v>
+        <v>403</v>
       </c>
       <c r="D63" t="s">
-        <v>426</v>
+        <v>404</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="D64" t="s">
-        <v>428</v>
+        <v>406</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>429</v>
+        <v>407</v>
       </c>
       <c r="D65" t="s">
-        <v>430</v>
+        <v>408</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>431</v>
+        <v>409</v>
       </c>
       <c r="D66" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>433</v>
+        <v>411</v>
       </c>
       <c r="D67" t="s">
-        <v>434</v>
+        <v>412</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>435</v>
+        <v>413</v>
       </c>
       <c r="D68" t="s">
-        <v>436</v>
+        <v>414</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>437</v>
+        <v>415</v>
       </c>
       <c r="D69" t="s">
-        <v>438</v>
+        <v>416</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>439</v>
+        <v>417</v>
       </c>
       <c r="D70" t="s">
-        <v>440</v>
+        <v>418</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>441</v>
+        <v>419</v>
       </c>
       <c r="D71" t="s">
-        <v>442</v>
+        <v>420</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>443</v>
+        <v>421</v>
       </c>
       <c r="D72" t="s">
-        <v>444</v>
+        <v>422</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>445</v>
+        <v>423</v>
       </c>
       <c r="D73" t="s">
-        <v>446</v>
+        <v>424</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>447</v>
+        <v>425</v>
       </c>
       <c r="D74" t="s">
-        <v>448</v>
+        <v>426</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>449</v>
+        <v>427</v>
       </c>
       <c r="D75" t="s">
-        <v>450</v>
+        <v>428</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>451</v>
+        <v>429</v>
       </c>
       <c r="D76" t="s">
-        <v>452</v>
+        <v>430</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>453</v>
+        <v>431</v>
       </c>
       <c r="D77" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>455</v>
+        <v>433</v>
       </c>
       <c r="D78" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D79" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>459</v>
+        <v>437</v>
       </c>
       <c r="D80" t="s">
-        <v>460</v>
+        <v>438</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>461</v>
+        <v>439</v>
       </c>
       <c r="D81" t="s">
-        <v>462</v>
+        <v>440</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>463</v>
+        <v>441</v>
       </c>
       <c r="D82" t="s">
-        <v>464</v>
+        <v>442</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>465</v>
+        <v>443</v>
       </c>
       <c r="D83" t="s">
-        <v>466</v>
+        <v>444</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>467</v>
+        <v>445</v>
       </c>
       <c r="D84" t="s">
-        <v>468</v>
+        <v>446</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>469</v>
+        <v>447</v>
+      </c>
+      <c r="D85" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="D86" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="D87" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="D88" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>476</v>
+        <v>455</v>
+      </c>
+      <c r="D89" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
       <c r="D90" t="s">
-        <v>478</v>
+        <v>458</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>479</v>
+        <v>459</v>
       </c>
       <c r="D91" t="s">
-        <v>480</v>
+        <v>460</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>481</v>
+        <v>461</v>
       </c>
       <c r="D92" t="s">
-        <v>482</v>
+        <v>462</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
       <c r="D93" t="s">
-        <v>484</v>
+        <v>464</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
       <c r="D94" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>487</v>
-      </c>
-      <c r="D95" t="s">
-        <v>488</v>
+        <v>467</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>489</v>
+        <v>468</v>
       </c>
       <c r="D96" t="s">
-        <v>490</v>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>470</v>
+      </c>
+      <c r="D97" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>491</v>
+        <v>472</v>
+      </c>
+      <c r="D98" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>492</v>
-      </c>
-      <c r="D99" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
       <c r="D100" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
       <c r="D101" t="s">
-        <v>497</v>
+        <v>478</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>498</v>
+        <v>479</v>
       </c>
       <c r="D102" t="s">
-        <v>499</v>
+        <v>480</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
       <c r="D103" t="s">
-        <v>501</v>
+        <v>482</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>502</v>
+        <v>483</v>
       </c>
       <c r="D104" t="s">
-        <v>503</v>
+        <v>484</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>504</v>
+        <v>485</v>
       </c>
       <c r="D105" t="s">
-        <v>505</v>
+        <v>486</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>506</v>
+        <v>487</v>
       </c>
       <c r="D106" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>508</v>
-      </c>
-      <c r="D107" t="s">
-        <v>509</v>
+        <v>488</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>510</v>
-      </c>
-      <c r="D108" t="s">
-        <v>511</v>
+        <v>489</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>512</v>
+        <v>490</v>
       </c>
       <c r="D109" t="s">
-        <v>513</v>
+        <v>491</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>514</v>
+        <v>492</v>
       </c>
       <c r="D110" t="s">
-        <v>515</v>
+        <v>493</v>
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>531</v>
+        <v>494</v>
       </c>
       <c r="D111" t="s">
-        <v>519</v>
+        <v>495</v>
       </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>532</v>
+        <v>496</v>
       </c>
       <c r="D112" t="s">
-        <v>520</v>
+        <v>497</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>533</v>
+        <v>498</v>
       </c>
       <c r="D113" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>534</v>
+        <v>500</v>
       </c>
       <c r="D114" t="s">
-        <v>538</v>
+        <v>501</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>535</v>
+        <v>502</v>
       </c>
       <c r="D115" t="s">
-        <v>539</v>
+        <v>503</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>536</v>
+        <v>504</v>
       </c>
       <c r="D116" t="s">
-        <v>540</v>
+        <v>505</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>537</v>
+        <v>506</v>
       </c>
       <c r="D117" t="s">
-        <v>541</v>
+        <v>507</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="D118" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="D119" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="D120" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="D121" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="D122" t="s">
-        <v>530</v>
+        <v>518</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="D123" t="s">
-        <v>523</v>
+        <v>514</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>532</v>
+      </c>
+      <c r="D124" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="D125" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>545</v>
+        <v>534</v>
       </c>
       <c r="D126" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="D127" t="s">
-        <v>547</v>
+        <v>539</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>520</v>
+      </c>
+      <c r="D128" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>515</v>
+      </c>
+      <c r="D129" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>523</v>
+      </c>
+      <c r="D130" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>524</v>
+      </c>
+      <c r="D131" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>525</v>
+      </c>
+      <c r="D132" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>522</v>
+      </c>
+      <c r="D133" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>540</v>
+      </c>
+      <c r="D135" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>543</v>
+      </c>
+      <c r="D136" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>544</v>
+      </c>
+      <c r="D137" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functional scenarios on shop apge
</commit_message>
<xml_diff>
--- a/ecommerse_automation_gurupreeth/project_documents_ANUSHA_shopPage.xlsx
+++ b/ecommerse_automation_gurupreeth/project_documents_ANUSHA_shopPage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\ECODERS_TESTING_FOLDER\project_management_tool_jira\ecommerse_automation_gurupreeth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BFC327-C4AA-4E14-9482-B5969A22CE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CEFF8B-DB6E-4EF0-B183-69AC07930FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="559">
   <si>
     <t>header elements</t>
   </si>
@@ -1705,6 +1705,30 @@
   </si>
   <si>
     <t>Single-Product | ECODERS</t>
+  </si>
+  <si>
+    <t>User Dashboard | ECODERS</t>
+  </si>
+  <si>
+    <t>About Us | ECODERS</t>
+  </si>
+  <si>
+    <t>Contact Us | ECODERS</t>
+  </si>
+  <si>
+    <t>Careers | ECODERS</t>
+  </si>
+  <si>
+    <t>All Blogs | ECODERS</t>
+  </si>
+  <si>
+    <t>Help |ECODERS</t>
+  </si>
+  <si>
+    <t>Privacy Policy | ECODERS</t>
+  </si>
+  <si>
+    <t>Terms of Service | ECODERS</t>
   </si>
 </sst>
 </file>
@@ -3038,10 +3062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3051,12 +3075,12 @@
     <col min="4" max="4" width="96.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>547</v>
       </c>
@@ -3064,1044 +3088,1084 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>306</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B22" t="s">
         <v>307</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D22" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>309</v>
-      </c>
-      <c r="D15" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>311</v>
-      </c>
-      <c r="D16" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>313</v>
-      </c>
-      <c r="D17" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>315</v>
-      </c>
-      <c r="D18" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>317</v>
-      </c>
-      <c r="D19" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>6</v>
-      </c>
-      <c r="B20" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>319</v>
-      </c>
-      <c r="D21" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>8</v>
-      </c>
-      <c r="B22" t="s">
-        <v>321</v>
-      </c>
-      <c r="D22" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="D23" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="D24" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="D25" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="D26" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="D27" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>333</v>
-      </c>
-      <c r="D28" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="D29" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="D30" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="D31" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>325</v>
+      </c>
+      <c r="D32" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>327</v>
+      </c>
+      <c r="D33" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>329</v>
+      </c>
+      <c r="D34" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>331</v>
+      </c>
+      <c r="D35" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>333</v>
+      </c>
+      <c r="D36" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37" t="s">
+        <v>335</v>
+      </c>
+      <c r="D37" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>337</v>
+      </c>
+      <c r="D38" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>17</v>
+      </c>
+      <c r="B39" t="s">
+        <v>339</v>
+      </c>
+      <c r="D39" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>18</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B40" t="s">
         <v>341</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D40" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>343</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D41" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>345</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D42" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>347</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D43" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>349</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D44" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>351</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D45" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>353</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D46" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>355</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D47" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>357</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D48" t="s">
         <v>358</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>359</v>
-      </c>
-      <c r="D41" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>361</v>
-      </c>
-      <c r="D42" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>363</v>
-      </c>
-      <c r="D43" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>365</v>
-      </c>
-      <c r="D44" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>367</v>
-      </c>
-      <c r="D45" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>369</v>
-      </c>
-      <c r="D46" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>371</v>
-      </c>
-      <c r="D47" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>373</v>
-      </c>
-      <c r="D48" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="D49" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="D50" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="D51" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="D52" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="D53" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="D54" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="D55" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="D56" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="D57" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="D58" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="D59" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="D60" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="D61" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="D62" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="D63" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="D64" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="D65" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="D66" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="D67" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="D68" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="D69" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
       <c r="D70" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
       <c r="D71" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="D72" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="D73" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="D74" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="D75" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="D76" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="D77" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="D78" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="D79" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="D80" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="D81" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="D82" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
       <c r="D83" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="D84" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="D85" t="s">
-        <v>448</v>
+        <v>432</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>449</v>
+        <v>433</v>
       </c>
       <c r="D86" t="s">
-        <v>450</v>
+        <v>434</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>451</v>
+        <v>435</v>
       </c>
       <c r="D87" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>453</v>
+        <v>437</v>
       </c>
       <c r="D88" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
       <c r="D89" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="D90" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
       <c r="D91" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
       <c r="D92" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="D93" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="D94" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>467</v>
+        <v>451</v>
+      </c>
+      <c r="D95" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="D96" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="D97" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="D98" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>474</v>
+        <v>459</v>
+      </c>
+      <c r="D99" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="D100" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
       <c r="D101" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="D102" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>481</v>
-      </c>
-      <c r="D103" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
       <c r="D104" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="D105" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
       <c r="D106" t="s">
-        <v>488</v>
+        <v>473</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>489</v>
+        <v>475</v>
+      </c>
+      <c r="D108" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="D109" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
       <c r="D110" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="D111" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
       <c r="D112" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="D113" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="D114" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>502</v>
-      </c>
-      <c r="D115" t="s">
-        <v>503</v>
+        <v>488</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>504</v>
-      </c>
-      <c r="D116" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="D117" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
       <c r="D118" t="s">
-        <v>509</v>
+        <v>493</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>510</v>
+        <v>494</v>
       </c>
       <c r="D119" t="s">
-        <v>511</v>
+        <v>495</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="D120" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>529</v>
+        <v>498</v>
       </c>
       <c r="D121" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>530</v>
+        <v>500</v>
       </c>
       <c r="D122" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>531</v>
+        <v>502</v>
       </c>
       <c r="D123" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>532</v>
+        <v>504</v>
       </c>
       <c r="D124" t="s">
-        <v>536</v>
+        <v>505</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>533</v>
+        <v>506</v>
       </c>
       <c r="D125" t="s">
-        <v>537</v>
+        <v>507</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>534</v>
+        <v>508</v>
       </c>
       <c r="D126" t="s">
-        <v>538</v>
+        <v>509</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>535</v>
+        <v>510</v>
       </c>
       <c r="D127" t="s">
-        <v>539</v>
+        <v>511</v>
       </c>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="D128" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>515</v>
+        <v>529</v>
       </c>
       <c r="D129" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="D130" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="D131" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="D132" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>522</v>
+        <v>533</v>
       </c>
       <c r="D133" t="s">
-        <v>521</v>
+        <v>537</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>534</v>
+      </c>
+      <c r="D134" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="D135" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>543</v>
+        <v>520</v>
       </c>
       <c r="D136" t="s">
-        <v>542</v>
+        <v>519</v>
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
+        <v>515</v>
+      </c>
+      <c r="D137" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>523</v>
+      </c>
+      <c r="D138" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>524</v>
+      </c>
+      <c r="D139" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>525</v>
+      </c>
+      <c r="D140" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>522</v>
+      </c>
+      <c r="D141" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>540</v>
+      </c>
+      <c r="D143" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>543</v>
+      </c>
+      <c r="D144" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
         <v>544</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D145" t="s">
         <v>545</v>
       </c>
     </row>

</xml_diff>

<commit_message>
functional scenarios on shop page
</commit_message>
<xml_diff>
--- a/ecommerse_automation_gurupreeth/project_documents_ANUSHA_shopPage.xlsx
+++ b/ecommerse_automation_gurupreeth/project_documents_ANUSHA_shopPage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\ECODERS_TESTING_FOLDER\project_management_tool_jira\ecommerse_automation_gurupreeth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CEFF8B-DB6E-4EF0-B183-69AC07930FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D51531-D386-49C8-9EAE-95965452825A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="560">
   <si>
     <t>header elements</t>
   </si>
@@ -1722,13 +1722,16 @@
     <t>All Blogs | ECODERS</t>
   </si>
   <si>
-    <t>Help |ECODERS</t>
-  </si>
-  <si>
     <t>Privacy Policy | ECODERS</t>
   </si>
   <si>
-    <t>Terms of Service | ECODERS</t>
+    <t>Help Center | ECODERS</t>
+  </si>
+  <si>
+    <t>Terms Of Service | ECODERS</t>
+  </si>
+  <si>
+    <t>Facebook - log in or sign up</t>
   </si>
 </sst>
 </file>
@@ -3065,7 +3068,7 @@
   <dimension ref="A1:D145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3135,17 +3138,22 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>558</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>